<commit_message>
added debug version of sat-map
</commit_message>
<xml_diff>
--- a/study/results/results.xlsx
+++ b/study/results/results.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexlong/Documents/Github/sat-map/study/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7E6DB6-94AF-094B-B38B-E57EE18EF241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42720047-C29C-8143-9D61-8918B112C661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="500" windowWidth="28340" windowHeight="19820" xr2:uid="{9FECDF54-19B7-7B40-B415-AEE003CB0F6B}"/>
+    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="26220" xr2:uid="{9FECDF54-19B7-7B40-B415-AEE003CB0F6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -177,13 +177,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -310,18 +311,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$11:$C$11</c:f>
+              <c:f>Sheet1!$A$12:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>h:mm</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.11520061728395062</c:v>
+                  <c:v>0.11187499999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.10516975308641976</c:v>
+                  <c:v>0.10451388888888891</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.12175925925925925</c:v>
+                  <c:v>0.11486111111111111</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -616,18 +617,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$11:$G$11</c:f>
+              <c:f>Sheet1!$E$12:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3.4444444444444446</c:v>
+                  <c:v>3.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.1111111111111107</c:v>
+                  <c:v>4.0999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.6666666666666665</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -918,18 +919,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$11:$K$11</c:f>
+              <c:f>Sheet1!$I$12:$K$12</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.88888888888888884</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2753,7 +2754,7 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2782,14 +2783,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2817,15 +2818,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3151,15 +3152,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60BC67A7-6793-4748-904D-AF2B016FE9CC}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.83203125" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.1640625" bestFit="1" customWidth="1"/>
@@ -3437,45 +3439,111 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
-        <f>AVERAGE(A2:A10)</f>
-        <v>0.11520061728395062</v>
-      </c>
-      <c r="B11" s="2">
-        <f t="shared" ref="B11:E11" si="0">AVERAGE(B2:B10)</f>
-        <v>0.10516975308641976</v>
-      </c>
-      <c r="C11" s="2">
-        <f t="shared" si="0"/>
-        <v>0.12175925925925925</v>
-      </c>
-      <c r="E11" s="4">
-        <f>AVERAGE(E2:E10)</f>
-        <v>3.4444444444444446</v>
-      </c>
-      <c r="F11" s="4">
-        <f t="shared" ref="F11:G11" si="1">AVERAGE(F2:F10)</f>
-        <v>4.1111111111111107</v>
-      </c>
-      <c r="G11" s="4">
-        <f t="shared" si="1"/>
-        <v>3.6666666666666665</v>
-      </c>
-      <c r="I11" s="5">
-        <f>((SUM(I2:I10))/9)</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="J11" s="5">
-        <f>((SUM(J2:J10))/9)</f>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="K11" s="5">
-        <f>((SUM(K2:K10))/9)</f>
-        <v>0.66666666666666663</v>
+      <c r="A11" s="1">
+        <v>8.1944444444444445E-2</v>
+      </c>
+      <c r="B11" s="1">
+        <v>9.8611111111111108E-2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>5.2777777777777778E-2</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <f>AVERAGE(A2:A11)</f>
+        <v>0.11187499999999999</v>
+      </c>
+      <c r="B12" s="2">
+        <f>AVERAGE(B2:B11)</f>
+        <v>0.10451388888888891</v>
+      </c>
+      <c r="C12" s="2">
+        <f>AVERAGE(C2:C11)</f>
+        <v>0.11486111111111111</v>
+      </c>
+      <c r="E12" s="4">
+        <f>AVERAGE(E2:E11)</f>
+        <v>3.6</v>
+      </c>
+      <c r="F12" s="4">
+        <f>AVERAGE(F2:F11)</f>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G12" s="4">
+        <f>AVERAGE(G2:G11)</f>
+        <v>3.7</v>
+      </c>
+      <c r="I12" s="5">
+        <f>((SUM(I2:I11))/10)</f>
+        <v>0.7</v>
+      </c>
+      <c r="J12" s="5">
+        <f>((SUM(J2:J11))/10)</f>
+        <v>0.9</v>
+      </c>
+      <c r="K12" s="5">
+        <f>((SUM(K2:K11))/10)</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <f>_xlfn.STDEV.S(A2:A11)</f>
+        <v>3.9836947444391903E-2</v>
+      </c>
+      <c r="B14" s="1">
+        <f>_xlfn.STDEV.S(B2:B11)</f>
+        <v>4.5042335005300985E-2</v>
+      </c>
+      <c r="C14" s="1">
+        <f>_xlfn.STDEV.S(C2:C11)</f>
+        <v>4.4060844575329675E-2</v>
+      </c>
+      <c r="E14" s="6">
+        <f>_xlfn.STDEV.S(E2:E11)</f>
+        <v>0.96609178307929622</v>
+      </c>
+      <c r="F14" s="6">
+        <f>_xlfn.STDEV.S(F2:F11)</f>
+        <v>0.73786478737262229</v>
+      </c>
+      <c r="G14" s="6">
+        <f>_xlfn.STDEV.S(G2:G11)</f>
+        <v>1.05934990547138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <f>A12-B12</f>
+        <v>7.3611111111110822E-3</v>
+      </c>
+      <c r="C16" s="1">
+        <f>C12-B12</f>
+        <v>1.0347222222222202E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>

</xml_diff>